<commit_message>
First Alpha release for Testing
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="23260" windowHeight="12580"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="23260" windowHeight="12580" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="93">
   <si>
     <t>Name</t>
   </si>
@@ -157,15 +157,6 @@
     <t>Please Provide the credential folder path for Oprchestrator Asset folder</t>
   </si>
   <si>
-    <t>BotFolder</t>
-  </si>
-  <si>
-    <t>Bot deployed orchestrator folder address, Where assets and other details are stored</t>
-  </si>
-  <si>
-    <t>SalesOrder</t>
-  </si>
-  <si>
     <t>TimeOut_M</t>
   </si>
   <si>
@@ -178,12 +169,6 @@
     <t>TimeOut_L</t>
   </si>
   <si>
-    <t>PORandom_Min</t>
-  </si>
-  <si>
-    <t>PORandom_Max</t>
-  </si>
-  <si>
     <t>Batch3_StartTime</t>
   </si>
   <si>
@@ -256,13 +241,67 @@
     <t>SME_Email</t>
   </si>
   <si>
-    <t>Email to be forwarded with urgent deliveries for manual handling</t>
-  </si>
-  <si>
-    <t>sourav.kumar1@linde.com</t>
-  </si>
-  <si>
-    <t>RPASupport</t>
+    <t>Data\Temp\RSK Sales Order Picked Mail Body.txt</t>
+  </si>
+  <si>
+    <t>RSK_SalesOrderPickedMailBody</t>
+  </si>
+  <si>
+    <t>MailProcessedFolder</t>
+  </si>
+  <si>
+    <t>Processed</t>
+  </si>
+  <si>
+    <t>MailNotProcessedFolder</t>
+  </si>
+  <si>
+    <t>Not Processed</t>
+  </si>
+  <si>
+    <t>SuccessfulEmailSubject</t>
+  </si>
+  <si>
+    <t>Consolidated Sales Order Tracker - Daily Update</t>
+  </si>
+  <si>
+    <t>SuccessEmailSubToRequestSender</t>
+  </si>
+  <si>
+    <t>RSK Sales Order Tracker</t>
+  </si>
+  <si>
+    <t>UrgentDeliveryMailSubject</t>
+  </si>
+  <si>
+    <t>Notice - SO is not created due to imminent delivery request</t>
+  </si>
+  <si>
+    <t>ConnectionName</t>
+  </si>
+  <si>
+    <t>SuccessEmailToRequestSenderSubject</t>
+  </si>
+  <si>
+    <t>RSK Sales Order Tracker for the SO request</t>
+  </si>
+  <si>
+    <t>RSK_UserBasedTrackerTempFile</t>
+  </si>
+  <si>
+    <t>Data\Temp\SOP_RSKTrackerTempFile.xlsx</t>
+  </si>
+  <si>
+    <t>Data\Temp\ConsolidatedEmailBody.txt</t>
+  </si>
+  <si>
+    <t>ConsolidatedMailBody</t>
+  </si>
+  <si>
+    <t>Data\Temp\RSKTracker_UserEmailBodyResponse.txt</t>
+  </si>
+  <si>
+    <t>RSKSenderWiseResponseMailBody</t>
   </si>
 </sst>
 </file>
@@ -649,10 +688,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z995"/>
+  <dimension ref="A1:Z990"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -699,10 +738,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
@@ -713,7 +752,7 @@
         <v>29</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>30</v>
@@ -725,7 +764,7 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>22</v>
@@ -743,122 +782,151 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A7" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B7" t="s">
-        <v>46</v>
+      <c r="A7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7">
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>51</v>
-      </c>
-      <c r="B8">
-        <v>10</v>
+        <v>50</v>
+      </c>
+      <c r="B8" s="7">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>52</v>
-      </c>
-      <c r="B9">
-        <v>99999</v>
+        <v>48</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>54</v>
-      </c>
-      <c r="B10">
-        <v>10</v>
+        <v>63</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>64</v>
       </c>
       <c r="C10" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>55</v>
-      </c>
-      <c r="B11" s="7">
-        <v>15</v>
+        <v>66</v>
+      </c>
+      <c r="B11" t="s">
+        <v>67</v>
       </c>
       <c r="C11" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A12" t="s">
-        <v>53</v>
-      </c>
-      <c r="B12" s="8" t="s">
+      <c r="A12" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B13" t="s">
         <v>75</v>
       </c>
-      <c r="C12" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A13" t="s">
-        <v>68</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C13" t="s">
-        <v>70</v>
-      </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A14" t="s">
-        <v>71</v>
+      <c r="A14" s="2" t="s">
+        <v>76</v>
       </c>
       <c r="B14" t="s">
-        <v>72</v>
-      </c>
-      <c r="C14" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A15" t="s">
-        <v>76</v>
-      </c>
-      <c r="B15" s="5" t="s">
+      <c r="A15" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C15" t="s">
-        <v>77</v>
+      <c r="B15" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+        <v>80</v>
+      </c>
+      <c r="B16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A17" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B17" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A18" t="s">
+        <v>85</v>
+      </c>
+      <c r="B18" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A19" t="s">
+        <v>87</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A20" t="s">
+        <v>90</v>
+      </c>
+      <c r="B20" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A21" t="s">
+        <v>92</v>
+      </c>
+      <c r="B21" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="23" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -1817,11 +1885,6 @@
     <row r="988" ht="14.25" customHeight="1"/>
     <row r="989" ht="14.25" customHeight="1"/>
     <row r="990" ht="14.25" customHeight="1"/>
-    <row r="991" ht="14.25" customHeight="1"/>
-    <row r="992" ht="14.25" customHeight="1"/>
-    <row r="993" ht="14.25" customHeight="1"/>
-    <row r="994" ht="14.25" customHeight="1"/>
-    <row r="995" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1833,8 +1896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -1884,7 +1947,7 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>23</v>
@@ -2017,35 +2080,35 @@
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B18">
         <v>10000</v>
       </c>
       <c r="C18" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B19">
         <v>5000</v>
       </c>
       <c r="C19" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B20">
         <v>30000</v>
       </c>
       <c r="C20" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
@@ -3024,10 +3087,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -3076,25 +3140,25 @@
     </row>
     <row r="2" spans="1:26" ht="42" customHeight="1">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -3102,61 +3166,81 @@
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B4" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B5" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B6" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B7" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B8" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>